<commit_message>
rombak tabel user & login pake nis. rombak tabel laporan. optimalisasi Form.
</commit_message>
<xml_diff>
--- a/public/user_import_template.xlsx
+++ b/public/user_import_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asche\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\sentrinaNIS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4823F39-9377-44B9-8E2A-8E168C997BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD16F21B-171A-4D2B-8220-9BCFB42250E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4DAEBCAA-1A37-41AC-A70A-DF408068E476}"/>
   </bookViews>
@@ -34,15 +34,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>email</t>
+    <t>password</t>
   </si>
   <si>
-    <t>password</t>
+    <t>kelompok</t>
+  </si>
+  <si>
+    <t>nis</t>
   </si>
 </sst>
 </file>
@@ -394,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7750ADC-FC25-491D-9E7D-93370716BCC4}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,15 +410,18 @@
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>